<commit_message>
Radial Decay and other changes
</commit_message>
<xml_diff>
--- a/FlaPyDisaster/Documentation/Hurricane/NOAA_NWS23_Inflow_Calcs.xlsx
+++ b/FlaPyDisaster/Documentation/Hurricane/NOAA_NWS23_Inflow_Calcs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14955" windowHeight="8205" tabRatio="719"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14955" windowHeight="6780" tabRatio="719"/>
   </bookViews>
   <sheets>
     <sheet name="InflowAngle" sheetId="14" r:id="rId1"/>
@@ -436,6 +436,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -494,13 +497,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -27425,6 +27429,12 @@
               </a:r>
             </a:p>
             <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                <a:t>Rmax = Radius of Maximum Winds</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
               <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
             </a:p>
             <a:p>
@@ -27575,6 +27585,21 @@
                       <m:rPr>
                         <m:nor/>
                       </m:rPr>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>(</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
                       <a:rPr lang="en-US" sz="1100" baseline="0">
                         <a:solidFill>
                           <a:schemeClr val="dk1"/>
@@ -27615,6 +27640,21 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
                       <m:t>Rmax</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
                     </m:r>
                     <m:r>
                       <m:rPr>
@@ -28575,7 +28615,7 @@
                       <m:rPr>
                         <m:nor/>
                       </m:rPr>
-                      <a:rPr lang="en-US" sz="1100" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
                         <a:solidFill>
                           <a:schemeClr val="dk1"/>
                         </a:solidFill>
@@ -28584,7 +28624,7 @@
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
-                      <m:t>0.0000896902</m:t>
+                      <m:t>−0.0000000592</m:t>
                     </m:r>
                     <m:r>
                       <m:rPr>
@@ -28629,13 +28669,13 @@
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
-                      <m:t> − </m:t>
+                      <m:t> </m:t>
                     </m:r>
                     <m:r>
                       <m:rPr>
                         <m:nor/>
                       </m:rPr>
-                      <a:rPr lang="en-US" sz="1100" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0">
                         <a:solidFill>
                           <a:schemeClr val="dk1"/>
                         </a:solidFill>
@@ -28644,7 +28684,22 @@
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
-                      <m:t>0.0036924418</m:t>
+                      <m:t>+ </m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:nor/>
+                      </m:rPr>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>0.0000019826</m:t>
                     </m:r>
                     <m:r>
                       <m:rPr>
@@ -28680,7 +28735,7 @@
                       <m:rPr>
                         <m:nor/>
                       </m:rPr>
-                      <a:rPr lang="en-US" sz="1100" baseline="0">
+                      <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
                         <a:solidFill>
                           <a:schemeClr val="dk1"/>
                         </a:solidFill>
@@ -28689,37 +28744,14 @@
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
-                      <m:t>+</m:t>
+                      <m:t>− 0.0000020198</m:t>
                     </m:r>
                     <m:r>
                       <m:rPr>
                         <m:nor/>
                       </m:rPr>
-                      <a:rPr lang="en-US" sz="1100" i="1" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="dk1"/>
-                        </a:solidFill>
-                        <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:rPr>
+                      <a:rPr lang="en-US"/>
                       <m:t> </m:t>
-                    </m:r>
-                    <m:r>
-                      <m:rPr>
-                        <m:nor/>
-                      </m:rPr>
-                      <a:rPr lang="en-US" sz="1100" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="dk1"/>
-                        </a:solidFill>
-                        <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:rPr>
-                      <m:t>0.0072307906</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -28764,7 +28796,7 @@
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
-                      <m:t> = 9.7043</m:t>
+                      <m:t> = 9.70435663</m:t>
                     </m:r>
                     <m:r>
                       <m:rPr>
@@ -28779,7 +28811,7 @@
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
-                      <m:t>566341</m:t>
+                      <m:t>41</m:t>
                     </m:r>
                     <m:r>
                       <m:rPr>
@@ -28921,6 +28953,12 @@
                         </m:r>
                       </m:sub>
                     </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>(</m:t>
+                    </m:r>
                     <m:sSup>
                       <m:sSupPr>
                         <m:ctrlPr>
@@ -28930,36 +28968,52 @@
                         </m:ctrlPr>
                       </m:sSupPr>
                       <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>(</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑑</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>−(3</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑅𝑚𝑎𝑥</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>))</m:t>
-                        </m:r>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑑</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−</m:t>
+                            </m:r>
+                            <m:d>
+                              <m:dPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:dPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>3</m:t>
+                                </m:r>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑅𝑚𝑎𝑥</m:t>
+                                </m:r>
+                              </m:e>
+                            </m:d>
+                          </m:e>
+                        </m:d>
                       </m:e>
                       <m:sup>
                         <m:r>
@@ -28974,7 +29028,7 @@
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>+ </m:t>
+                      <m:t>)+ </m:t>
                     </m:r>
                     <m:sSub>
                       <m:sSubPr>
@@ -29044,7 +29098,7 @@
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
-                          <m:t>(</m:t>
+                          <m:t>((</m:t>
                         </m:r>
                         <m:r>
                           <a:rPr lang="en-US" sz="1100" b="0" i="1">
@@ -29120,7 +29174,7 @@
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
-                      <m:t>+ </m:t>
+                      <m:t>)+ </m:t>
                     </m:r>
                     <m:sSub>
                       <m:sSubPr>
@@ -29243,11 +29297,9 @@
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
             <a:p>
-              <a:pPr/>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
             <a:p>
-              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100"/>
                 <a:t>Still to do: Find the distance of PhiMax from</a:t>
@@ -29320,6 +29372,12 @@
               <a:r>
                 <a:rPr lang="en-US" sz="1100" baseline="0"/>
                 <a:t>Final Regression: Given Rmax and Distance from Hurricane center, Calculate Inflow Angle (Phi)</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                <a:t>Rmax = Radius of Maximum Winds</a:t>
               </a:r>
             </a:p>
             <a:p>
@@ -29427,19 +29485,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>𝑏= </a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>"</a:t>
+                <a:t>𝑏= "(</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" i="0" baseline="0">
@@ -29463,7 +29509,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t> ∗ Rmax</a:t>
+                <a:t> ∗ Rmax)</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" i="0" baseline="0">
@@ -29882,10 +29928,10 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>𝑥_3= "</a:t>
+                <a:t>𝑥_3= </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1100" i="0" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="dk1"/>
                   </a:solidFill>
@@ -29894,7 +29940,19 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>0.0000896902</a:t>
+                <a:t>"</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>−0.0000000592</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
@@ -29930,7 +29988,31 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t> − 0.0036924418</a:t>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>+ </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>0.0000019826</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
@@ -29954,18 +30036,28 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t> + 0.0072307906</a:t>
+                <a:t> </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1100" i="0" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
                   <a:solidFill>
                     <a:schemeClr val="dk1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
+                <a:t>− 0.0000020198</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" i="0"/>
                 <a:t>"</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" b="0" baseline="0">
@@ -29984,7 +30076,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>"c = 9.70</a:t>
+                <a:t>"c = 9.704356</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" i="0" baseline="0">
@@ -29996,7 +30088,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>43566341ln(</a:t>
+                <a:t>6341ln(</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
@@ -30042,7 +30134,7 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑃ℎ𝑖= 𝑥_3 〖(𝑑−(3𝑅𝑚𝑎𝑥))〗^3+ </a:t>
+                <a:t>𝑃ℎ𝑖= 𝑥_3 ((𝑑−(3𝑅𝑚𝑎𝑥))^3)+ </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
@@ -30054,16 +30146,14 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>𝑥_2 〖(𝑑−(3𝑅𝑚𝑎𝑥))〗^2+ 𝑥_1 (𝑑−(3𝑅𝑚𝑎𝑥))+𝑐</a:t>
+                <a:t>𝑥_2 〖((𝑑−(3𝑅𝑚𝑎𝑥))〗^2)+ 𝑥_1 (𝑑−(3𝑅𝑚𝑎𝑥))+𝑐</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
             <a:p>
-              <a:pPr/>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
             <a:p>
-              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100"/>
                 <a:t>Still to do: Find the distance of PhiMax from</a:t>
@@ -34096,59 +34186,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AR24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
       <c r="L2" s="2"/>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4" t="s">
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
     </row>
     <row r="3" spans="2:44" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
@@ -34174,8 +34264,8 @@
         <v>17</v>
       </c>
       <c r="L3" s="3"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
       <c r="P3" s="1" t="s">
         <v>5</v>
       </c>
@@ -34775,51 +34865,51 @@
       </c>
     </row>
     <row r="14" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="N14" s="4" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="N14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
-      <c r="W14" s="4" t="s">
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="4"/>
-      <c r="AB14" s="4"/>
-      <c r="AC14" s="4"/>
-      <c r="AD14" s="4"/>
-      <c r="AE14" s="4"/>
-      <c r="AF14" s="4"/>
-      <c r="AG14" s="4"/>
-      <c r="AH14" s="4"/>
-      <c r="AI14" s="4"/>
-      <c r="AJ14" s="4"/>
-      <c r="AK14" s="4"/>
-      <c r="AL14" s="4"/>
-      <c r="AM14" s="4"/>
-      <c r="AN14" s="4"/>
-      <c r="AO14" s="4"/>
-      <c r="AP14" s="4"/>
-      <c r="AQ14" s="4"/>
-      <c r="AR14" s="4"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="5"/>
+      <c r="AI14" s="5"/>
+      <c r="AJ14" s="5"/>
+      <c r="AK14" s="5"/>
+      <c r="AL14" s="5"/>
+      <c r="AM14" s="5"/>
+      <c r="AN14" s="5"/>
+      <c r="AO14" s="5"/>
+      <c r="AP14" s="5"/>
+      <c r="AQ14" s="5"/>
+      <c r="AR14" s="5"/>
     </row>
     <row r="15" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -34950,7 +35040,7 @@
       <c r="D16" s="1">
         <v>1.1453</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="4">
         <v>-5.9200000000000001E-8</v>
       </c>
       <c r="F16" s="1">
@@ -35099,7 +35189,7 @@
       <c r="D17" s="1">
         <v>1.45363</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="4">
         <v>1.9825999999999999E-6</v>
       </c>
       <c r="F17" s="1">
@@ -35244,7 +35334,7 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1">
+      <c r="E18" s="4">
         <v>-2.0198000000000001E-6</v>
       </c>
       <c r="F18" s="1">
@@ -36152,8 +36242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39745,8 +39835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:J1048576"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>